<commit_message>
Modificaciones se agrega la final Champions 2024 03042025 1747
</commit_message>
<xml_diff>
--- a/final_champions_league.xlsx
+++ b/final_champions_league.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\ciencia_de_datos\streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{41807022-0CB3-47D5-9E9D-BF9AF74F0363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41475A1-F2F1-400A-8835-7D2BEBF367E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{918EBB11-7182-4429-870D-20B537C9D4A2}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="205">
   <si>
     <t>season</t>
   </si>
@@ -635,6 +635,9 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>2023-24</t>
   </si>
 </sst>
 </file>
@@ -1495,9 +1498,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E504BEC6-E9DA-4456-9DCB-2D2F3FFEFF3E}">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4553,6 +4559,50 @@
         <v>203</v>
       </c>
     </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>138</v>
+      </c>
+      <c r="G70" t="s">
+        <v>132</v>
+      </c>
+      <c r="H70" t="s">
+        <v>47</v>
+      </c>
+      <c r="I70" t="s">
+        <v>48</v>
+      </c>
+      <c r="J70" t="s">
+        <v>49</v>
+      </c>
+      <c r="K70">
+        <v>86212</v>
+      </c>
+      <c r="L70" t="s">
+        <v>202</v>
+      </c>
+      <c r="M70" t="s">
+        <v>203</v>
+      </c>
+      <c r="N70" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N69" xr:uid="{E504BEC6-E9DA-4456-9DCB-2D2F3FFEFF3E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>